<commit_message>
Update Especificação + UC de Exercicios
-Alteração no UC Gestor de Exercicios;
-Alteração minima na especificação do gestor de utilizador;
-Especificacao do gestor de Exercícios (90%);
</commit_message>
<xml_diff>
--- a/Diagramas de UC e Especificações Textuais/3-Especificação do Gestor de Utilizadores.xlsx
+++ b/Diagramas de UC e Especificações Textuais/3-Especificação do Gestor de Utilizadores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RS\Documents\GitHub\EAW_MEI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RS\Documents\GitHub\EAW_MEI\Diagramas de UC e Especificações Textuais\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -392,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -856,11 +856,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -909,7 +992,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -920,7 +1002,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -934,8 +1015,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -974,8 +1053,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -985,276 +1062,309 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1538,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J95" sqref="J95"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:XFD99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,51 +1665,51 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="86"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="97"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="89"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="100"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="89"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="100"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="92"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="103"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="104" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1"/>
@@ -1618,7 +1728,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="163"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="3">
         <v>1</v>
       </c>
@@ -1630,12 +1740,12 @@
       <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="100" t="s">
+      <c r="H7" s="89" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="163"/>
+      <c r="B8" s="105"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3">
@@ -1647,10 +1757,10 @@
       <c r="G8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="100"/>
+      <c r="H8" s="89"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="163"/>
+      <c r="B9" s="105"/>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
       <c r="E9" s="3">
@@ -1662,10 +1772,10 @@
       <c r="G9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="100"/>
+      <c r="H9" s="89"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="163"/>
+      <c r="B10" s="105"/>
       <c r="C10" s="5">
         <v>4</v>
       </c>
@@ -1677,12 +1787,12 @@
       <c r="G10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="109" t="s">
+      <c r="H10" s="90" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="163"/>
+      <c r="B11" s="105"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="5">
@@ -1694,34 +1804,34 @@
       <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="164"/>
+      <c r="H11" s="91"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="163"/>
-      <c r="C12" s="152"/>
-      <c r="D12" s="154"/>
-      <c r="E12" s="156">
+      <c r="B12" s="105"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="110">
         <v>6</v>
       </c>
-      <c r="F12" s="158" t="s">
+      <c r="F12" s="112" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="160" t="s">
+      <c r="G12" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="164"/>
+      <c r="H12" s="91"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="163"/>
-      <c r="C13" s="153"/>
-      <c r="D13" s="155"/>
-      <c r="E13" s="157"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="161"/>
-      <c r="H13" s="164"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="91"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="163"/>
+      <c r="B14" s="105"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
       <c r="E14" s="5">
@@ -1733,10 +1843,10 @@
       <c r="G14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="164"/>
+      <c r="H14" s="91"/>
     </row>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="163"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="7">
@@ -1746,10 +1856,10 @@
         <v>14</v>
       </c>
       <c r="G15" s="8"/>
-      <c r="H15" s="164"/>
+      <c r="H15" s="91"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="118" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1761,12 +1871,12 @@
       <c r="E16" s="10"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="101" t="s">
+      <c r="H16" s="121" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="148"/>
+      <c r="B17" s="119"/>
       <c r="C17" s="17"/>
       <c r="D17" s="18"/>
       <c r="E17" s="19" t="s">
@@ -1778,44 +1888,44 @@
       <c r="G17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="102"/>
+      <c r="H17" s="122"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="148"/>
-      <c r="C18" s="151"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="106" t="s">
+      <c r="B18" s="119"/>
+      <c r="C18" s="117"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="107" t="s">
+      <c r="F18" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="105" t="s">
+      <c r="G18" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="102"/>
+      <c r="H18" s="122"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="148"/>
-      <c r="C19" s="151"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="102"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="125"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="122"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="149"/>
+      <c r="B20" s="120"/>
       <c r="C20" s="15"/>
       <c r="D20" s="16"/>
       <c r="E20" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="165" t="s">
+      <c r="F20" s="78" t="s">
         <v>29</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="103"/>
+      <c r="H20" s="123"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
@@ -1830,56 +1940,56 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="84" t="s">
+      <c r="C22" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="85"/>
-      <c r="E22" s="85"/>
-      <c r="F22" s="86"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="97"/>
       <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="89"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="100"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="87" t="s">
+      <c r="C24" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="88"/>
-      <c r="E24" s="88"/>
-      <c r="F24" s="89"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="100"/>
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="90"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="92"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="102"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="103"/>
       <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
-      <c r="B26" s="147" t="s">
+      <c r="B26" s="118" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="1"/>
@@ -1900,7 +2010,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
-      <c r="B27" s="148"/>
+      <c r="B27" s="119"/>
       <c r="C27" s="22">
         <v>1</v>
       </c>
@@ -1914,7 +2024,7 @@
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="148"/>
+      <c r="B28" s="119"/>
       <c r="C28" s="3">
         <v>2</v>
       </c>
@@ -1926,12 +2036,12 @@
       <c r="G28" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="100" t="s">
+      <c r="H28" s="89" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="148"/>
+      <c r="B29" s="119"/>
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="28">
@@ -1943,10 +2053,10 @@
       <c r="G29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="100"/>
+      <c r="H29" s="89"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="148"/>
+      <c r="B30" s="119"/>
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
       <c r="E30" s="28">
@@ -1958,10 +2068,10 @@
       <c r="G30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="100"/>
+      <c r="H30" s="89"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="148"/>
+      <c r="B31" s="119"/>
       <c r="C31" s="3"/>
       <c r="D31" s="4"/>
       <c r="E31" s="28">
@@ -1973,10 +2083,10 @@
       <c r="G31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="100"/>
+      <c r="H31" s="89"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="149"/>
+      <c r="B32" s="120"/>
       <c r="C32" s="25"/>
       <c r="D32" s="26"/>
       <c r="E32" s="29">
@@ -1986,7 +2096,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="26"/>
-      <c r="H32" s="150"/>
+      <c r="H32" s="126"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21"/>
@@ -2002,77 +2112,77 @@
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21"/>
-      <c r="B34" s="62" t="s">
+      <c r="B34" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="84" t="s">
+      <c r="C34" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="86"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="97"/>
       <c r="I34" s="21"/>
       <c r="J34" s="21"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21"/>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="87" t="s">
+      <c r="C35" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="89"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="100"/>
       <c r="I35" s="21"/>
       <c r="J35" s="21"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21"/>
-      <c r="B36" s="62" t="s">
+      <c r="B36" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="87" t="s">
+      <c r="C36" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="88"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="89"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="100"/>
       <c r="I36" s="21"/>
       <c r="J36" s="21"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21"/>
-      <c r="B37" s="62" t="s">
+      <c r="B37" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="90" t="s">
+      <c r="C37" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="91"/>
-      <c r="E37" s="91"/>
-      <c r="F37" s="92"/>
+      <c r="D37" s="102"/>
+      <c r="E37" s="102"/>
+      <c r="F37" s="103"/>
       <c r="I37" s="21"/>
       <c r="J37" s="21"/>
     </row>
     <row r="38" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21"/>
-      <c r="B38" s="93" t="s">
+      <c r="B38" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="54"/>
-      <c r="D38" s="36" t="s">
+      <c r="C38" s="50"/>
+      <c r="D38" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36" t="s">
+      <c r="E38" s="34"/>
+      <c r="F38" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="36" t="s">
+      <c r="G38" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="37" t="s">
+      <c r="H38" s="36" t="s">
         <v>8</v>
       </c>
       <c r="I38" s="21"/>
@@ -2080,19 +2190,19 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
-      <c r="B39" s="94"/>
-      <c r="C39" s="55">
+      <c r="B39" s="129"/>
+      <c r="C39" s="51">
         <v>1</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D39" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40" t="s">
+      <c r="E39" s="37"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="95" t="s">
+      <c r="H39" s="134" t="s">
         <v>10</v>
       </c>
       <c r="I39" s="21"/>
@@ -2100,49 +2210,49 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="146"/>
-      <c r="D40" s="145"/>
-      <c r="E40" s="144">
+      <c r="B40" s="129"/>
+      <c r="C40" s="127"/>
+      <c r="D40" s="150"/>
+      <c r="E40" s="149">
         <v>2</v>
       </c>
-      <c r="F40" s="143" t="s">
+      <c r="F40" s="148" t="s">
         <v>86</v>
       </c>
-      <c r="G40" s="139" t="s">
+      <c r="G40" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="H40" s="96"/>
+      <c r="H40" s="135"/>
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
-      <c r="B41" s="94"/>
-      <c r="C41" s="146"/>
-      <c r="D41" s="145"/>
-      <c r="E41" s="144"/>
-      <c r="F41" s="143"/>
-      <c r="G41" s="139"/>
-      <c r="H41" s="128"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="127"/>
+      <c r="D41" s="150"/>
+      <c r="E41" s="149"/>
+      <c r="F41" s="148"/>
+      <c r="G41" s="144"/>
+      <c r="H41" s="136"/>
       <c r="I41" s="21"/>
       <c r="J41" s="21"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="94"/>
-      <c r="C42" s="56">
+      <c r="B42" s="129"/>
+      <c r="C42" s="52">
         <v>3</v>
       </c>
-      <c r="D42" s="48" t="s">
+      <c r="D42" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="47"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48" t="s">
+      <c r="E42" s="45"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="H42" s="135" t="s">
+      <c r="H42" s="131" t="s">
         <v>13</v>
       </c>
       <c r="I42" s="21"/>
@@ -2150,126 +2260,126 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="94"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="47">
+      <c r="B43" s="129"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="45">
         <v>4</v>
       </c>
-      <c r="F43" s="48" t="s">
+      <c r="F43" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="48" t="s">
+      <c r="G43" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="H43" s="136"/>
+      <c r="H43" s="132"/>
       <c r="I43" s="21"/>
       <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="94"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="47">
+      <c r="B44" s="129"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="45">
         <v>5</v>
       </c>
-      <c r="F44" s="48" t="s">
+      <c r="F44" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="G44" s="48" t="s">
+      <c r="G44" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="137"/>
+      <c r="H44" s="133"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="94"/>
-      <c r="C45" s="57">
+      <c r="B45" s="129"/>
+      <c r="C45" s="53">
         <v>6</v>
       </c>
-      <c r="D45" s="43" t="s">
+      <c r="D45" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="42"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43" t="s">
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="H45" s="129" t="s">
+      <c r="H45" s="137" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="94"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="42">
+      <c r="B46" s="129"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="40">
         <v>7</v>
       </c>
-      <c r="F46" s="43" t="s">
+      <c r="F46" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="G46" s="43" t="s">
+      <c r="G46" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="H46" s="130"/>
+      <c r="H46" s="138"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="94"/>
-      <c r="C47" s="133"/>
-      <c r="D47" s="142"/>
-      <c r="E47" s="141">
+      <c r="B47" s="129"/>
+      <c r="C47" s="167"/>
+      <c r="D47" s="147"/>
+      <c r="E47" s="146">
         <v>8</v>
       </c>
-      <c r="F47" s="140" t="s">
+      <c r="F47" s="145" t="s">
         <v>47</v>
       </c>
-      <c r="G47" s="117" t="s">
+      <c r="G47" s="165" t="s">
         <v>11</v>
       </c>
-      <c r="H47" s="130"/>
+      <c r="H47" s="138"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="94"/>
-      <c r="C48" s="133"/>
-      <c r="D48" s="142"/>
-      <c r="E48" s="141"/>
-      <c r="F48" s="140"/>
-      <c r="G48" s="118"/>
-      <c r="H48" s="130"/>
+      <c r="B48" s="129"/>
+      <c r="C48" s="167"/>
+      <c r="D48" s="147"/>
+      <c r="E48" s="146"/>
+      <c r="F48" s="145"/>
+      <c r="G48" s="166"/>
+      <c r="H48" s="138"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="94"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="42">
+      <c r="B49" s="129"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="40">
         <v>9</v>
       </c>
-      <c r="F49" s="43" t="s">
+      <c r="F49" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="G49" s="43" t="s">
+      <c r="G49" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="130"/>
+      <c r="H49" s="138"/>
     </row>
     <row r="50" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="134"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="44">
+      <c r="B50" s="130"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="42">
         <v>10</v>
       </c>
-      <c r="F50" s="46" t="s">
+      <c r="F50" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="45"/>
-      <c r="H50" s="131"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="139"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="97" t="s">
+      <c r="B51" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="C51" s="59" t="s">
+      <c r="C51" s="55" t="s">
         <v>49</v>
       </c>
       <c r="D51" s="11" t="s">
@@ -2278,13 +2388,13 @@
       <c r="E51" s="10"/>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
-      <c r="H51" s="101" t="s">
+      <c r="H51" s="121" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="98"/>
-      <c r="C52" s="60"/>
+      <c r="B52" s="141"/>
+      <c r="C52" s="56"/>
       <c r="D52" s="18"/>
       <c r="E52" s="19" t="s">
         <v>50</v>
@@ -2295,99 +2405,99 @@
       <c r="G52" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H52" s="102"/>
+      <c r="H52" s="122"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="98"/>
-      <c r="C53" s="138"/>
-      <c r="D53" s="105"/>
-      <c r="E53" s="106" t="s">
+      <c r="B53" s="141"/>
+      <c r="C53" s="143"/>
+      <c r="D53" s="116"/>
+      <c r="E53" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="F53" s="107" t="s">
+      <c r="F53" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="G53" s="132" t="s">
+      <c r="G53" s="156" t="s">
         <v>11</v>
       </c>
-      <c r="H53" s="102"/>
+      <c r="H53" s="122"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="98"/>
-      <c r="C54" s="138"/>
-      <c r="D54" s="105"/>
-      <c r="E54" s="106"/>
-      <c r="F54" s="107"/>
-      <c r="G54" s="132"/>
-      <c r="H54" s="102"/>
+      <c r="B54" s="141"/>
+      <c r="C54" s="143"/>
+      <c r="D54" s="116"/>
+      <c r="E54" s="125"/>
+      <c r="F54" s="124"/>
+      <c r="G54" s="156"/>
+      <c r="H54" s="122"/>
     </row>
     <row r="55" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="99"/>
-      <c r="C55" s="61"/>
+      <c r="B55" s="142"/>
+      <c r="C55" s="57"/>
       <c r="D55" s="16"/>
       <c r="E55" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F55" s="165" t="s">
+      <c r="F55" s="78" t="s">
         <v>53</v>
       </c>
       <c r="G55" s="16"/>
-      <c r="H55" s="103"/>
+      <c r="H55" s="123"/>
     </row>
     <row r="56" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="63"/>
+      <c r="B56" s="59"/>
       <c r="C56" s="30"/>
       <c r="E56" s="30"/>
     </row>
     <row r="57" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="62" t="s">
+      <c r="B57" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="84" t="s">
+      <c r="C57" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="D57" s="85"/>
-      <c r="E57" s="85"/>
-      <c r="F57" s="86"/>
+      <c r="D57" s="96"/>
+      <c r="E57" s="96"/>
+      <c r="F57" s="97"/>
     </row>
     <row r="58" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="62" t="s">
+      <c r="B58" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="87" t="s">
+      <c r="C58" s="98" t="s">
         <v>71</v>
       </c>
-      <c r="D58" s="88"/>
-      <c r="E58" s="88"/>
-      <c r="F58" s="89"/>
+      <c r="D58" s="99"/>
+      <c r="E58" s="99"/>
+      <c r="F58" s="100"/>
     </row>
     <row r="59" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="62" t="s">
+      <c r="B59" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="87" t="s">
+      <c r="C59" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="88"/>
-      <c r="E59" s="88"/>
-      <c r="F59" s="89"/>
+      <c r="D59" s="99"/>
+      <c r="E59" s="99"/>
+      <c r="F59" s="100"/>
     </row>
     <row r="60" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="62" t="s">
+      <c r="B60" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="90" t="s">
+      <c r="C60" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="D60" s="91"/>
-      <c r="E60" s="91"/>
-      <c r="F60" s="92"/>
+      <c r="D60" s="102"/>
+      <c r="E60" s="102"/>
+      <c r="F60" s="103"/>
     </row>
     <row r="61" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="97" t="s">
+      <c r="B61" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="51"/>
+      <c r="C61" s="47"/>
       <c r="D61" s="1" t="s">
         <v>5</v>
       </c>
@@ -2403,8 +2513,8 @@
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="98"/>
-      <c r="C62" s="52">
+      <c r="B62" s="141"/>
+      <c r="C62" s="48">
         <v>1</v>
       </c>
       <c r="D62" s="22" t="s">
@@ -2416,8 +2526,8 @@
       <c r="H62" s="24"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="98"/>
-      <c r="C63" s="53">
+      <c r="B63" s="141"/>
+      <c r="C63" s="49">
         <v>2</v>
       </c>
       <c r="D63" s="4" t="s">
@@ -2428,13 +2538,13 @@
       <c r="G63" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H63" s="127" t="s">
+      <c r="H63" s="153" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="98"/>
-      <c r="C64" s="53"/>
+      <c r="B64" s="141"/>
+      <c r="C64" s="49"/>
       <c r="D64" s="4"/>
       <c r="E64" s="32">
         <v>3</v>
@@ -2445,82 +2555,82 @@
       <c r="G64" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="H64" s="128"/>
+      <c r="H64" s="136"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="98"/>
-      <c r="C65" s="69">
+      <c r="B65" s="141"/>
+      <c r="C65" s="65">
         <v>4</v>
       </c>
-      <c r="D65" s="43" t="s">
+      <c r="D65" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="E65" s="65"/>
-      <c r="F65" s="66"/>
-      <c r="G65" s="66" t="s">
+      <c r="E65" s="61"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="H65" s="129" t="s">
+      <c r="H65" s="137" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="98"/>
-      <c r="C66" s="115"/>
-      <c r="D66" s="123"/>
-      <c r="E66" s="121">
+      <c r="B66" s="141"/>
+      <c r="C66" s="163"/>
+      <c r="D66" s="154"/>
+      <c r="E66" s="159">
         <v>5</v>
       </c>
-      <c r="F66" s="119" t="s">
+      <c r="F66" s="157" t="s">
         <v>57</v>
       </c>
-      <c r="G66" s="168" t="s">
+      <c r="G66" s="161" t="s">
         <v>11</v>
       </c>
-      <c r="H66" s="130"/>
+      <c r="H66" s="138"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="98"/>
-      <c r="C67" s="116"/>
-      <c r="D67" s="124"/>
-      <c r="E67" s="122"/>
-      <c r="F67" s="120"/>
-      <c r="G67" s="169"/>
-      <c r="H67" s="130"/>
+      <c r="B67" s="141"/>
+      <c r="C67" s="164"/>
+      <c r="D67" s="155"/>
+      <c r="E67" s="160"/>
+      <c r="F67" s="158"/>
+      <c r="G67" s="162"/>
+      <c r="H67" s="138"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="98"/>
-      <c r="C68" s="69"/>
-      <c r="D68" s="43"/>
-      <c r="E68" s="67">
+      <c r="B68" s="141"/>
+      <c r="C68" s="65"/>
+      <c r="D68" s="41"/>
+      <c r="E68" s="63">
         <v>6</v>
       </c>
-      <c r="F68" s="43" t="s">
+      <c r="F68" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="G68" s="43" t="s">
+      <c r="G68" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="H68" s="130"/>
+      <c r="H68" s="138"/>
     </row>
     <row r="69" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="99"/>
-      <c r="C69" s="70"/>
-      <c r="D69" s="66"/>
-      <c r="E69" s="65">
+      <c r="B69" s="142"/>
+      <c r="C69" s="66"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="61">
         <v>7</v>
       </c>
-      <c r="F69" s="68" t="s">
+      <c r="F69" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="G69" s="66"/>
-      <c r="H69" s="131"/>
+      <c r="G69" s="62"/>
+      <c r="H69" s="139"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="97" t="s">
+      <c r="B70" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="C70" s="59" t="s">
+      <c r="C70" s="55" t="s">
         <v>60</v>
       </c>
       <c r="D70" s="11" t="s">
@@ -2531,111 +2641,113 @@
       <c r="G70" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H70" s="125" t="s">
+      <c r="H70" s="151" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="71" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="99"/>
-      <c r="C71" s="64"/>
+      <c r="B71" s="142"/>
+      <c r="C71" s="60"/>
       <c r="D71" s="14"/>
       <c r="E71" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F71" s="167" t="s">
+      <c r="F71" s="80" t="s">
         <v>62</v>
       </c>
       <c r="G71" s="14"/>
-      <c r="H71" s="126"/>
-    </row>
-    <row r="72" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="H71" s="152"/>
+    </row>
+    <row r="72" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G72" s="180"/>
+    </row>
     <row r="73" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="62" t="s">
+      <c r="B73" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="84" t="s">
+      <c r="C73" s="185" t="s">
         <v>73</v>
       </c>
-      <c r="D73" s="85"/>
-      <c r="E73" s="85"/>
-      <c r="F73" s="85"/>
-      <c r="G73" s="49"/>
-      <c r="H73" s="50"/>
+      <c r="D73" s="186"/>
+      <c r="E73" s="186"/>
+      <c r="F73" s="187"/>
+      <c r="G73" s="179"/>
+      <c r="H73" s="179"/>
     </row>
     <row r="74" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="62" t="s">
+      <c r="B74" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="87" t="s">
+      <c r="C74" s="175" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="88"/>
-      <c r="E74" s="88"/>
-      <c r="F74" s="88"/>
-      <c r="G74" s="34"/>
-      <c r="H74" s="41"/>
+      <c r="D74" s="176"/>
+      <c r="E74" s="176"/>
+      <c r="F74" s="177"/>
+      <c r="G74" s="179"/>
+      <c r="H74" s="179"/>
     </row>
     <row r="75" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="62" t="s">
+      <c r="B75" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C75" s="87" t="s">
+      <c r="C75" s="181" t="s">
         <v>40</v>
       </c>
-      <c r="D75" s="88"/>
-      <c r="E75" s="88"/>
-      <c r="F75" s="88"/>
-      <c r="G75" s="34"/>
-      <c r="H75" s="41"/>
+      <c r="D75" s="99"/>
+      <c r="E75" s="99"/>
+      <c r="F75" s="100"/>
+      <c r="G75" s="179"/>
+      <c r="H75" s="179"/>
     </row>
     <row r="76" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="62" t="s">
+      <c r="B76" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="90" t="s">
+      <c r="C76" s="182" t="s">
         <v>75</v>
       </c>
-      <c r="D76" s="91"/>
-      <c r="E76" s="91"/>
-      <c r="F76" s="91"/>
-      <c r="G76" s="77"/>
-      <c r="H76" s="78"/>
+      <c r="D76" s="183"/>
+      <c r="E76" s="183"/>
+      <c r="F76" s="184"/>
+      <c r="G76" s="179"/>
+      <c r="H76" s="179"/>
     </row>
     <row r="77" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="97" t="s">
+      <c r="B77" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="73"/>
-      <c r="D77" s="73" t="s">
+      <c r="C77" s="69"/>
+      <c r="D77" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="73"/>
-      <c r="F77" s="73" t="s">
+      <c r="E77" s="69"/>
+      <c r="F77" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="G77" s="73" t="s">
+      <c r="G77" s="178" t="s">
         <v>7</v>
       </c>
-      <c r="H77" s="73" t="s">
+      <c r="H77" s="178" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="98"/>
-      <c r="C78" s="72">
+      <c r="B78" s="141"/>
+      <c r="C78" s="68">
         <v>1</v>
       </c>
-      <c r="D78" s="74" t="s">
+      <c r="D78" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="E78" s="75"/>
-      <c r="F78" s="76"/>
-      <c r="G78" s="76"/>
-      <c r="H78" s="79"/>
+      <c r="E78" s="71"/>
+      <c r="F78" s="72"/>
+      <c r="G78" s="72"/>
+      <c r="H78" s="73"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="98"/>
-      <c r="C79" s="53">
+      <c r="B79" s="141"/>
+      <c r="C79" s="49">
         <v>2</v>
       </c>
       <c r="D79" s="4" t="s">
@@ -2646,13 +2758,13 @@
       <c r="G79" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H79" s="100" t="s">
+      <c r="H79" s="89" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="98"/>
-      <c r="C80" s="53"/>
+      <c r="B80" s="141"/>
+      <c r="C80" s="49"/>
       <c r="D80" s="4"/>
       <c r="E80" s="3">
         <v>3</v>
@@ -2663,11 +2775,11 @@
       <c r="G80" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H80" s="100"/>
+      <c r="H80" s="89"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="98"/>
-      <c r="C81" s="53"/>
+      <c r="B81" s="141"/>
+      <c r="C81" s="49"/>
       <c r="D81" s="4"/>
       <c r="E81" s="3">
         <v>4</v>
@@ -2678,11 +2790,11 @@
       <c r="G81" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H81" s="100"/>
+      <c r="H81" s="89"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="98"/>
-      <c r="C82" s="71">
+      <c r="B82" s="141"/>
+      <c r="C82" s="67">
         <v>5</v>
       </c>
       <c r="D82" s="6" t="s">
@@ -2693,13 +2805,13 @@
       <c r="G82" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H82" s="108" t="s">
+      <c r="H82" s="169" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="98"/>
-      <c r="C83" s="71"/>
+      <c r="B83" s="141"/>
+      <c r="C83" s="67"/>
       <c r="D83" s="6"/>
       <c r="E83" s="5">
         <v>6</v>
@@ -2710,35 +2822,35 @@
       <c r="G83" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H83" s="108"/>
+      <c r="H83" s="169"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="98"/>
-      <c r="C84" s="110"/>
-      <c r="D84" s="111"/>
-      <c r="E84" s="112">
+      <c r="B84" s="141"/>
+      <c r="C84" s="170"/>
+      <c r="D84" s="171"/>
+      <c r="E84" s="172">
         <v>7</v>
       </c>
-      <c r="F84" s="113" t="s">
+      <c r="F84" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="G84" s="114" t="s">
+      <c r="G84" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="H84" s="108"/>
+      <c r="H84" s="169"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="98"/>
-      <c r="C85" s="110"/>
-      <c r="D85" s="111"/>
-      <c r="E85" s="112"/>
-      <c r="F85" s="113"/>
-      <c r="G85" s="114"/>
-      <c r="H85" s="108"/>
+      <c r="B85" s="141"/>
+      <c r="C85" s="170"/>
+      <c r="D85" s="171"/>
+      <c r="E85" s="172"/>
+      <c r="F85" s="173"/>
+      <c r="G85" s="174"/>
+      <c r="H85" s="169"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="98"/>
-      <c r="C86" s="71"/>
+      <c r="B86" s="141"/>
+      <c r="C86" s="67"/>
       <c r="D86" s="6"/>
       <c r="E86" s="5">
         <v>8</v>
@@ -2749,11 +2861,11 @@
       <c r="G86" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H86" s="108"/>
+      <c r="H86" s="169"/>
     </row>
     <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="99"/>
-      <c r="C87" s="80"/>
+      <c r="B87" s="142"/>
+      <c r="C87" s="74"/>
       <c r="D87" s="8"/>
       <c r="E87" s="7">
         <v>9</v>
@@ -2762,13 +2874,13 @@
         <v>14</v>
       </c>
       <c r="G87" s="8"/>
-      <c r="H87" s="109"/>
+      <c r="H87" s="90"/>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="97" t="s">
+      <c r="B88" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="81" t="s">
+      <c r="C88" s="75" t="s">
         <v>24</v>
       </c>
       <c r="D88" s="11" t="s">
@@ -2777,13 +2889,13 @@
       <c r="E88" s="10"/>
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
-      <c r="H88" s="101" t="s">
+      <c r="H88" s="121" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="98"/>
-      <c r="C89" s="82"/>
+      <c r="B89" s="141"/>
+      <c r="C89" s="76"/>
       <c r="D89" s="18"/>
       <c r="E89" s="19" t="s">
         <v>26</v>
@@ -2794,90 +2906,90 @@
       <c r="G89" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H89" s="102"/>
+      <c r="H89" s="122"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="98"/>
-      <c r="C90" s="104"/>
-      <c r="D90" s="105"/>
-      <c r="E90" s="106" t="s">
+      <c r="B90" s="141"/>
+      <c r="C90" s="168"/>
+      <c r="D90" s="116"/>
+      <c r="E90" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="F90" s="107" t="s">
+      <c r="F90" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="G90" s="105" t="s">
+      <c r="G90" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="H90" s="102"/>
+      <c r="H90" s="122"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="98"/>
-      <c r="C91" s="104"/>
-      <c r="D91" s="105"/>
-      <c r="E91" s="106"/>
-      <c r="F91" s="107"/>
-      <c r="G91" s="105"/>
-      <c r="H91" s="102"/>
+      <c r="B91" s="141"/>
+      <c r="C91" s="168"/>
+      <c r="D91" s="116"/>
+      <c r="E91" s="125"/>
+      <c r="F91" s="124"/>
+      <c r="G91" s="116"/>
+      <c r="H91" s="122"/>
     </row>
     <row r="92" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="99"/>
-      <c r="C92" s="83"/>
+      <c r="B92" s="142"/>
+      <c r="C92" s="77"/>
       <c r="D92" s="16"/>
       <c r="E92" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F92" s="165" t="s">
+      <c r="F92" s="78" t="s">
         <v>77</v>
       </c>
       <c r="G92" s="16"/>
-      <c r="H92" s="103"/>
+      <c r="H92" s="123"/>
     </row>
     <row r="93" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="94" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="62" t="s">
+      <c r="B94" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C94" s="84" t="s">
+      <c r="C94" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="D94" s="85"/>
-      <c r="E94" s="85"/>
-      <c r="F94" s="86"/>
+      <c r="D94" s="96"/>
+      <c r="E94" s="96"/>
+      <c r="F94" s="97"/>
     </row>
     <row r="95" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="62" t="s">
+      <c r="B95" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C95" s="87" t="s">
+      <c r="C95" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="D95" s="88"/>
-      <c r="E95" s="88"/>
-      <c r="F95" s="89"/>
+      <c r="D95" s="99"/>
+      <c r="E95" s="99"/>
+      <c r="F95" s="100"/>
     </row>
     <row r="96" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="62" t="s">
+      <c r="B96" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C96" s="87" t="s">
+      <c r="C96" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="D96" s="88"/>
-      <c r="E96" s="88"/>
-      <c r="F96" s="89"/>
+      <c r="D96" s="99"/>
+      <c r="E96" s="99"/>
+      <c r="F96" s="100"/>
     </row>
     <row r="97" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="166" t="s">
+      <c r="B97" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="C97" s="90"/>
-      <c r="D97" s="91"/>
-      <c r="E97" s="91"/>
-      <c r="F97" s="92"/>
+      <c r="C97" s="101"/>
+      <c r="D97" s="102"/>
+      <c r="E97" s="102"/>
+      <c r="F97" s="103"/>
     </row>
     <row r="98" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B98" s="147" t="s">
+      <c r="B98" s="118" t="s">
         <v>4</v>
       </c>
       <c r="C98" s="1"/>
@@ -2896,94 +3008,94 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="148"/>
-      <c r="C99" s="170"/>
-      <c r="D99" s="171"/>
-      <c r="E99" s="172">
+      <c r="B99" s="119"/>
+      <c r="C99" s="81"/>
+      <c r="D99" s="82"/>
+      <c r="E99" s="83">
         <v>1</v>
       </c>
-      <c r="F99" s="171" t="s">
+      <c r="F99" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="G99" s="171" t="s">
+      <c r="G99" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="H99" s="173" t="s">
+      <c r="H99" s="92" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="148"/>
-      <c r="C100" s="170">
+      <c r="B100" s="119"/>
+      <c r="C100" s="81">
         <v>2</v>
       </c>
-      <c r="D100" s="171" t="s">
+      <c r="D100" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="E100" s="172"/>
-      <c r="F100" s="171"/>
-      <c r="G100" s="171" t="s">
+      <c r="E100" s="83"/>
+      <c r="F100" s="82"/>
+      <c r="G100" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="H100" s="174"/>
+      <c r="H100" s="93"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="148"/>
-      <c r="C101" s="170"/>
-      <c r="D101" s="171"/>
-      <c r="E101" s="172">
+      <c r="B101" s="119"/>
+      <c r="C101" s="81"/>
+      <c r="D101" s="82"/>
+      <c r="E101" s="83">
         <v>3</v>
       </c>
-      <c r="F101" s="171" t="s">
+      <c r="F101" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="G101" s="171" t="s">
+      <c r="G101" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="H101" s="174"/>
+      <c r="H101" s="93"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="148"/>
-      <c r="C102" s="170"/>
-      <c r="D102" s="171"/>
-      <c r="E102" s="172">
+      <c r="B102" s="119"/>
+      <c r="C102" s="81"/>
+      <c r="D102" s="82"/>
+      <c r="E102" s="83">
         <v>4</v>
       </c>
-      <c r="F102" s="171" t="s">
+      <c r="F102" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="G102" s="171" t="s">
+      <c r="G102" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="H102" s="174"/>
+      <c r="H102" s="93"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="148"/>
-      <c r="C103" s="170"/>
-      <c r="D103" s="171"/>
-      <c r="E103" s="172">
+      <c r="B103" s="119"/>
+      <c r="C103" s="81"/>
+      <c r="D103" s="82"/>
+      <c r="E103" s="83">
         <v>5</v>
       </c>
-      <c r="F103" s="175" t="s">
+      <c r="F103" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="G103" s="171" t="s">
+      <c r="G103" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="H103" s="174"/>
+      <c r="H103" s="93"/>
     </row>
     <row r="104" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B104" s="12"/>
-      <c r="C104" s="176"/>
-      <c r="D104" s="177"/>
-      <c r="E104" s="178">
+      <c r="C104" s="85"/>
+      <c r="D104" s="86"/>
+      <c r="E104" s="87">
         <v>6</v>
       </c>
-      <c r="F104" s="179" t="s">
+      <c r="F104" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="G104" s="177"/>
-      <c r="H104" s="180"/>
+      <c r="G104" s="86"/>
+      <c r="H104" s="94"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="21"/>
@@ -3023,37 +3135,48 @@
     </row>
   </sheetData>
   <mergeCells count="89">
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="H10:H15"/>
-    <mergeCell ref="H99:H104"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="H16:H20"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="H28:H32"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C94:F94"/>
+    <mergeCell ref="C95:F95"/>
+    <mergeCell ref="C96:F96"/>
+    <mergeCell ref="C97:F97"/>
+    <mergeCell ref="B98:B103"/>
+    <mergeCell ref="B88:B92"/>
+    <mergeCell ref="H79:H81"/>
+    <mergeCell ref="H88:H92"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="G90:G91"/>
+    <mergeCell ref="H82:H87"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="G84:G85"/>
+    <mergeCell ref="B77:B87"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="C75:F75"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C76:F76"/>
+    <mergeCell ref="B61:B69"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="H70:H71"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="H65:H69"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C58:F58"/>
+    <mergeCell ref="C59:F59"/>
+    <mergeCell ref="C60:F60"/>
     <mergeCell ref="B38:B50"/>
     <mergeCell ref="H42:H44"/>
     <mergeCell ref="H39:H41"/>
@@ -3070,48 +3193,37 @@
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="E40:E41"/>
     <mergeCell ref="D40:D41"/>
-    <mergeCell ref="H70:H71"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="H65:H69"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C58:F58"/>
-    <mergeCell ref="C59:F59"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C76:F76"/>
-    <mergeCell ref="B61:B69"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="C74:F74"/>
-    <mergeCell ref="C75:F75"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B88:B92"/>
-    <mergeCell ref="H79:H81"/>
-    <mergeCell ref="H88:H92"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="G90:G91"/>
-    <mergeCell ref="H82:H87"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="G84:G85"/>
-    <mergeCell ref="B77:B87"/>
-    <mergeCell ref="C94:F94"/>
-    <mergeCell ref="C95:F95"/>
-    <mergeCell ref="C96:F96"/>
-    <mergeCell ref="C97:F97"/>
-    <mergeCell ref="B98:B103"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="H16:H20"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="H28:H32"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="H99:H104"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>